<commit_message>
adding select options for team
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="160">
   <si>
     <t>id</t>
   </si>
@@ -81,57 +81,60 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 6</t>
   </si>
   <si>
+    <t>Team One</t>
+  </si>
+  <si>
+    <t>Tag 6</t>
+  </si>
+  <si>
+    <t>Team Member 2</t>
+  </si>
+  <si>
+    <t>Team Member 1, Team Member 2, Team Member 8</t>
+  </si>
+  <si>
+    <t>Category 3</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+  <si>
+    <t>Idea 4</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 4</t>
+  </si>
+  <si>
+    <t>Team 4</t>
+  </si>
+  <si>
+    <t>Tag 4</t>
+  </si>
+  <si>
+    <t>Team Member 1, Team Member 2, Team Member 6</t>
+  </si>
+  <si>
+    <t>Idea 5</t>
+  </si>
+  <si>
+    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 5</t>
+  </si>
+  <si>
+    <t>Team 5</t>
+  </si>
+  <si>
+    <t>Tag 5</t>
+  </si>
+  <si>
+    <t>Team Member 1, Team Member 2, Team Member 7</t>
+  </si>
+  <si>
+    <t>Idea 6</t>
+  </si>
+  <si>
     <t>Team 6</t>
   </si>
   <si>
-    <t>Tag 6</t>
-  </si>
-  <si>
-    <t>Team Member 2</t>
-  </si>
-  <si>
-    <t>Team Member 1, Team Member 2, Team Member 8</t>
-  </si>
-  <si>
-    <t>Category 3</t>
-  </si>
-  <si>
-    <t>ongoing</t>
-  </si>
-  <si>
-    <t>Idea 4</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 4</t>
-  </si>
-  <si>
-    <t>Team 4</t>
-  </si>
-  <si>
-    <t>Tag 4</t>
-  </si>
-  <si>
-    <t>Team Member 1, Team Member 2, Team Member 6</t>
-  </si>
-  <si>
-    <t>Idea 5</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 5</t>
-  </si>
-  <si>
-    <t>Team 5</t>
-  </si>
-  <si>
-    <t>Tag 5</t>
-  </si>
-  <si>
-    <t>Team Member 1, Team Member 2, Team Member 7</t>
-  </si>
-  <si>
-    <t>Idea 6</t>
-  </si>
-  <si>
     <t>Idea 7</t>
   </si>
   <si>
@@ -171,15 +174,15 @@
     <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Neque convallis a cras semper auctor. Lorem ipsum dolor sit amet consectetur adipiscing. Morbi tincidunt ornare massa eget egestas purus viverra accumsan. Non pulvinar neque laoreet suspendisse. Aliquam vestibulum morbi blandit cursus risus. Aenean et tortor at risus viverra adipiscing. Id venenatis a condimentum vitae sapien pellentesque habitant morbi. Feugiat in ante metus dictum at tempor. Pretium quam vulputate dignissim suspendisse in. Description 9</t>
   </si>
   <si>
-    <t>Team 9</t>
-  </si>
-  <si>
     <t>Tag 9</t>
   </si>
   <si>
     <t>Team Member 1, Team Member 2, Team Member 11</t>
   </si>
   <si>
+    <t>dropped</t>
+  </si>
+  <si>
     <t>Idea 10</t>
   </si>
   <si>
@@ -484,9 +487,6 @@
   </si>
   <si>
     <t>Team Name</t>
-  </si>
-  <si>
-    <t>Team One</t>
   </si>
   <si>
     <t>Team Two</t>
@@ -620,7 +620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" hidden="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" ht="12.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>11</v>
       </c>
@@ -684,7 +684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" hidden="1" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" ht="12.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -791,7 +791,7 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
@@ -817,16 +817,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="2">
         <v>43897</v>
@@ -835,10 +835,10 @@
         <v>43906</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
         <v>17</v>
@@ -849,16 +849,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F9" s="2">
         <v>43898</v>
@@ -867,45 +867,45 @@
         <v>43907</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
+    <row r="10" ht="12.8" customHeight="1" hidden="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>43899</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>43908</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I10" t="s">
         <v>53</v>
       </c>
       <c r="J10" t="s">
         <v>25</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -913,16 +913,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F11" s="2">
         <v>43900</v>
@@ -934,7 +934,7 @@
         <v>23</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J11" t="s">
         <v>17</v>
@@ -945,16 +945,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F12" s="2">
         <v>43901</v>
@@ -966,7 +966,7 @@
         <v>23</v>
       </c>
       <c r="I12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J12" t="s">
         <v>25</v>
@@ -977,16 +977,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F13" s="2">
         <v>43902</v>
@@ -995,10 +995,10 @@
         <v>43911</v>
       </c>
       <c r="H13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J13" t="s">
         <v>17</v>
@@ -1009,16 +1009,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F14" s="2">
         <v>43903</v>
@@ -1027,10 +1027,10 @@
         <v>43912</v>
       </c>
       <c r="H14" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J14" t="s">
         <v>25</v>
@@ -1041,16 +1041,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F15" s="2">
         <v>43904</v>
@@ -1059,10 +1059,10 @@
         <v>43913</v>
       </c>
       <c r="H15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
         <v>25</v>
@@ -1073,16 +1073,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F16" s="2">
         <v>43905</v>
@@ -1091,13 +1091,13 @@
         <v>43914</v>
       </c>
       <c r="H16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1105,16 +1105,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F17" s="2">
         <v>43906</v>
@@ -1123,10 +1123,10 @@
         <v>43915</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J17" t="s">
         <v>25</v>
@@ -1137,16 +1137,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F18" s="2">
         <v>43907</v>
@@ -1155,13 +1155,13 @@
         <v>43916</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J18" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1169,16 +1169,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F19" s="2">
         <v>43908</v>
@@ -1187,13 +1187,13 @@
         <v>43917</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I19" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1201,16 +1201,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F20" s="2">
         <v>43909</v>
@@ -1219,10 +1219,10 @@
         <v>43918</v>
       </c>
       <c r="H20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J20" t="s">
         <v>25</v>
@@ -1233,16 +1233,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E21" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F21" s="2">
         <v>43910</v>
@@ -1251,13 +1251,13 @@
         <v>43919</v>
       </c>
       <c r="H21" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1265,16 +1265,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C22" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F22" s="2">
         <v>43911</v>
@@ -1283,10 +1283,10 @@
         <v>43920</v>
       </c>
       <c r="H22" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J22" t="s">
         <v>25</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="23" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C23" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E23" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F23" s="3">
         <v>43891.34726608796</v>
@@ -1309,24 +1309,24 @@
         <v>43900.77083333333</v>
       </c>
       <c r="H23" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I23" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J23" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E24" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F24" s="3">
         <v>43913</v>
@@ -1335,24 +1335,24 @@
         <v>43922</v>
       </c>
       <c r="H24" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I24" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" ht="13.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F25" s="3">
         <v>43891.34726608796</v>
@@ -1361,27 +1361,27 @@
         <v>43900.77083333333</v>
       </c>
       <c r="H25" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" ht="12.8" customHeight="1" hidden="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D27" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F27" s="3">
         <v>43891.34726608796</v>
@@ -1390,13 +1390,13 @@
         <v>43900.77083333333</v>
       </c>
       <c r="H27" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I27" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J27" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1429,10 +1429,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -1446,7 +1446,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1460,7 +1460,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -1471,10 +1471,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1485,10 +1485,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -1499,10 +1499,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1513,10 +1513,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -1527,10 +1527,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -1541,10 +1541,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -1555,10 +1555,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1569,10 +1569,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D11">
         <v>4</v>
@@ -1583,10 +1583,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1597,10 +1597,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D13">
         <v>4</v>
@@ -1611,10 +1611,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1625,10 +1625,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D15">
         <v>4</v>
@@ -1686,7 +1686,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" ht="12.8" customHeight="1" hidden="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" hidden="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>